<commit_message>
fix bag & remove logs
</commit_message>
<xml_diff>
--- a/backend/uploads/statistics.xlsx
+++ b/backend/uploads/statistics.xlsx
@@ -397,15 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -413,13 +412,10 @@
         <v>first_name</v>
       </c>
       <c r="B1" t="str">
-        <v>last_name</v>
+        <v>email</v>
       </c>
       <c r="C1" t="str">
-        <v>department</v>
-      </c>
-      <c r="D1" t="str">
-        <v>totalSum</v>
+        <v>gender</v>
       </c>
     </row>
     <row r="2">
@@ -427,51 +423,20 @@
         <v>Alexia</v>
       </c>
       <c r="B2" t="str">
-        <v>Alessandone</v>
+        <v>aalessandone18@clickbank.net</v>
       </c>
       <c r="C2" t="str">
-        <v>Automotive</v>
-      </c>
-      <c r="D2" t="str">
-        <v>$803.83</v>
+        <v>Female</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>Nadiya</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Cawdron</v>
-      </c>
       <c r="C3" t="str">
-        <v>Automotive</v>
-      </c>
-      <c r="D3" t="str">
-        <v>$943.42</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Samson</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Whiterod</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Automotive</v>
-      </c>
-      <c r="D4" t="str">
-        <v>$366.09</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="D5" t="str">
-        <v>$2113.34</v>
+        <v>$803.83</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>